<commit_message>
added advanced tasks data
</commit_message>
<xml_diff>
--- a/src/test/resources/data/tasks_data.xlsx
+++ b/src/test/resources/data/tasks_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="simple tasks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>task name</t>
   </si>
@@ -28,6 +28,75 @@
   </si>
   <si>
     <t>create automation basePage class</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>due date</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>07.11.21</t>
+  </si>
+  <si>
+    <t>5.11.2021</t>
+  </si>
+  <si>
+    <t>10.11.21</t>
+  </si>
+  <si>
+    <t>16.11.2021</t>
+  </si>
+  <si>
+    <t>29.10.21</t>
+  </si>
+  <si>
+    <t>5.1.2022</t>
+  </si>
+  <si>
+    <t>create a new advanced task</t>
+  </si>
+  <si>
+    <t>creating a new advanced task for testing purposes</t>
+  </si>
+  <si>
+    <t>rzf</t>
+  </si>
+  <si>
+    <t>create a new page class</t>
+  </si>
+  <si>
+    <t>create a new page class derived from base</t>
+  </si>
+  <si>
+    <t>rzf, automation</t>
+  </si>
+  <si>
+    <t>add comments</t>
+  </si>
+  <si>
+    <t>add loging support</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>create negative scenarios</t>
+  </si>
+  <si>
+    <t>create at least 5 negative scenarios</t>
+  </si>
+  <si>
+    <t>add prjoject to github</t>
   </si>
 </sst>
 </file>
@@ -43,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -53,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -84,10 +159,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -428,12 +512,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
removed due date column in 'advanced tasks' sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/tasks_data.xlsx
+++ b/src/test/resources/data/tasks_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>task name</t>
   </si>
@@ -512,16 +512,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D4" sqref="D4:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -638,16 +745,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>